<commit_message>
1. Created structure ( styleworker, imageworker, creator )
</commit_message>
<xml_diff>
--- a/ExcelCard.xlsx
+++ b/ExcelCard.xlsx
@@ -149,15 +149,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>400000</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>200000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>143153</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>581222</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>838175</xdr:rowOff>
+      <xdr:rowOff>638175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -174,7 +174,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="400000" y="200000"/>
+          <a:off x="0" y="0"/>
           <a:ext cx="1762125" cy="638175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -187,15 +187,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>420000</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>130000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>277453</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>695522</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>806275</xdr:rowOff>
+      <xdr:rowOff>676275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -212,7 +212,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="420000" y="130000"/>
+          <a:off x="0" y="0"/>
           <a:ext cx="1876425" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>

<commit_message>
1. sorted on Classes
</commit_message>
<xml_diff>
--- a/ExcelCard.xlsx
+++ b/ExcelCard.xlsx
@@ -35,7 +35,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -66,11 +66,6 @@
     </border>
     <border>
       <left style="medium"/>
-      <right style="thin"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="thin"/>
       <bottom style="thin"/>
     </border>
     <border>
@@ -80,24 +75,17 @@
       <right style="medium"/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="medium"/>
-    </border>
-    <border>
-      <left style="thin"/>
       <right style="medium"/>
       <bottom style="thin"/>
     </border>
     <border>
       <left style="medium"/>
-      <right style="thin"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
       <right style="medium"/>
       <bottom style="medium"/>
     </border>
@@ -105,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
@@ -116,30 +104,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -149,15 +134,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>420000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>150000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>581222</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>163153</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>638175</xdr:rowOff>
+      <xdr:rowOff>788175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -174,7 +159,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="420000" y="150000"/>
           <a:ext cx="1762125" cy="638175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -187,15 +172,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>400000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>130000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>695522</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>257453</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>676275</xdr:rowOff>
+      <xdr:rowOff>806275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -212,7 +197,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="400000" y="130000"/>
           <a:ext cx="1876425" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -227,7 +212,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -288,18 +273,14 @@
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
     </row>
-    <row r="12">
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
1. fillCells working 2. Created new Class with options ( fill sel )
</commit_message>
<xml_diff>
--- a/ExcelCard.xlsx
+++ b/ExcelCard.xlsx
@@ -12,19 +12,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="3">
+  <si>
+    <t>Жирный Центр Item</t>
+  </si>
+  <si>
+    <t>Жирный лево Item</t>
+  </si>
+  <si>
+    <t>final left</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
@@ -125,6 +155,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -234,43 +306,71 @@
       <c r="D3" s="6"/>
     </row>
     <row r="4" ht="35.25" customHeight="true">
-      <c r="B4" s="7"/>
+      <c r="B4" s="31" t="s">
+        <v>0</v>
+      </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
     </row>
     <row r="5">
-      <c r="B5" s="10"/>
+      <c r="B5" s="32" t="s">
+        <v>1</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
     </row>
     <row r="6">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>0</v>
+      </c>
       <c r="D6" s="15"/>
     </row>
     <row r="7">
-      <c r="B7" s="16"/>
+      <c r="B7" s="34" t="s">
+        <v>1</v>
+      </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
+      <c r="D7" s="40" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
+      <c r="B8" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
-      <c r="B9" s="22"/>
+      <c r="B9" s="36" t="s">
+        <v>1</v>
+      </c>
       <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
+      <c r="D9" s="42" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
+      <c r="C10" s="43" t="s">
+        <v>2</v>
+      </c>
       <c r="D10" s="27"/>
     </row>
     <row r="11">
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
+      <c r="B11" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>2</v>
+      </c>
       <c r="D11" s="30"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Card is filled out (with params from Item )
</commit_message>
<xml_diff>
--- a/ExcelCard.xlsx
+++ b/ExcelCard.xlsx
@@ -12,15 +12,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="3">
-  <si>
-    <t>Жирный Центр Item</t>
-  </si>
-  <si>
-    <t>Жирный лево Item</t>
-  </si>
-  <si>
-    <t>final left</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Саморезы гипс/металл	3.5x25</t>
+  </si>
+  <si>
+    <t>Marking</t>
+  </si>
+  <si>
+    <t>YZP</t>
+  </si>
+  <si>
+    <t>РАЗМЕР/Size</t>
+  </si>
+  <si>
+    <t>Кол-во в упак/шт.</t>
+  </si>
+  <si>
+    <t>Вес упак Кг/Kgs</t>
+  </si>
+  <si>
+    <t>ORDER:</t>
+  </si>
+  <si>
+    <t>3.5x25</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Шт / PCS</t>
+  </si>
+  <si>
+    <t>Кг/Kgs</t>
+  </si>
+  <si>
+    <t>Сделано в КНР</t>
+  </si>
+  <si>
+    <t>2155695PL</t>
   </si>
 </sst>
 </file>
@@ -123,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
@@ -156,13 +186,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
@@ -181,9 +211,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
@@ -305,7 +332,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" ht="35.25" customHeight="true">
+    <row r="4" ht="50.0" customHeight="true">
       <c r="B4" s="31" t="s">
         <v>0</v>
       </c>
@@ -316,60 +343,58 @@
       <c r="B5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="33" t="s">
+        <v>2</v>
+      </c>
       <c r="D5" s="12"/>
     </row>
     <row r="6">
-      <c r="B6" s="33" t="s">
-        <v>1</v>
+      <c r="B6" s="34" t="s">
+        <v>3</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D6" s="15"/>
     </row>
     <row r="7">
-      <c r="B7" s="34" t="s">
-        <v>1</v>
-      </c>
+      <c r="B7" s="16"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="D7" s="18"/>
     </row>
     <row r="8">
       <c r="B8" s="35" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="36" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="23"/>
-      <c r="D9" s="42" t="s">
-        <v>2</v>
+      <c r="D9" s="41" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="25"/>
-      <c r="C10" s="43" t="s">
-        <v>2</v>
+      <c r="C10" s="42" t="s">
+        <v>11</v>
       </c>
       <c r="D10" s="27"/>
     </row>
     <row r="11">
       <c r="B11" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>12</v>
       </c>
       <c r="D11" s="30"/>
     </row>

</xml_diff>